<commit_message>
Make Final Products in Libraries sheet -> True
</commit_message>
<xml_diff>
--- a/Plant Parts/Plant Parts.xlsx
+++ b/Plant Parts/Plant Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE60BFD-FC9D-4043-9CBF-6C83E35349A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50834A8-E767-44F6-8FDF-DBF6D3307795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23209,11 +23209,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -23222,6 +23217,11 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23678,8 +23678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -23753,14 +23753,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="45.95" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="53" t="s">
         <v>7536</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -24017,13 +24017,13 @@
       <c r="D15" s="41" t="s">
         <v>1397</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="50" t="s">
         <v>7538</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="51" t="s">
         <v>7534</v>
       </c>
       <c r="H15" s="41" t="s">
@@ -24045,25 +24045,25 @@
       <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="49" t="s">
         <v>7550</v>
       </c>
       <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="49" t="s">
         <v>7539</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>1397</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="50" t="s">
         <v>7540</v>
       </c>
       <c r="F16" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="55" t="s">
+      <c r="G16" s="52" t="s">
         <v>7541</v>
       </c>
       <c r="H16" s="41" t="s">
@@ -24097,7 +24097,7 @@
       <c r="D17" s="41" t="s">
         <v>1397</v>
       </c>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="50" t="s">
         <v>7545</v>
       </c>
       <c r="F17" s="41" t="s">
@@ -24137,13 +24137,13 @@
       <c r="D18" s="20" t="s">
         <v>1397</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="50" t="s">
         <v>7546</v>
       </c>
       <c r="F18" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="55" t="s">
+      <c r="G18" s="52" t="s">
         <v>7548</v>
       </c>
       <c r="H18" s="41" t="s">
@@ -25647,8 +25647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -26141,18 +26141,18 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="49" t="s">
         <v>7537</v>
       </c>
       <c r="B14" s="21"/>
       <c r="D14" s="21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="41" t="s">
         <v>7501</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="49" t="s">
         <v>7555</v>
       </c>
       <c r="H14" s="18"/>

</xml_diff>

<commit_message>
Create library for Plant CDSs
</commit_message>
<xml_diff>
--- a/Plant Parts/Plant Parts.xlsx
+++ b/Plant Parts/Plant Parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50834A8-E767-44F6-8FDF-DBF6D3307795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{233AF336-2B10-4C73-8EF7-1B2680E406D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7630" uniqueCount="7558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7633" uniqueCount="7559">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22788,6 +22788,9 @@
   </si>
   <si>
     <t>CDS that confers hygromycin resistance when expressed with a plant promoter and terminator</t>
+  </si>
+  <si>
+    <t>Plant CDSs</t>
   </si>
 </sst>
 </file>
@@ -23679,7 +23682,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -25648,7 +25651,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -26174,14 +26177,21 @@
       <c r="X14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75">
+      <c r="A15" t="s">
+        <v>7558</v>
+      </c>
       <c r="B15" s="21"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>7501</v>
+      </c>
       <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="G15" s="18" t="s">
+        <v>7556</v>
+      </c>
       <c r="H15" s="21"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>

</xml_diff>

<commit_message>
Add plant parts and flanking sequences
</commit_message>
<xml_diff>
--- a/Plant Parts/Plant Parts.xlsx
+++ b/Plant Parts/Plant Parts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\iGEM-distribution_2\Plant Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{233AF336-2B10-4C73-8EF7-1B2680E406D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D7F441-9C2B-41AB-8342-F2C3B32BC006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7633" uniqueCount="7559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7792" uniqueCount="7595">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22704,18 +22704,6 @@
     <t>Plant Parts</t>
   </si>
   <si>
-    <t>Nikolaos Delkis</t>
-  </si>
-  <si>
-    <t>BBa_K1467101</t>
-  </si>
-  <si>
-    <t>Source = BBa_K1467101, Golden Gate compatible</t>
-  </si>
-  <si>
-    <t>This collection contains useful parts (shuttle vectors, promoters, UTRs, CDSs, terminators) for plant genetic engineering</t>
-  </si>
-  <si>
     <t>Plant promoters</t>
   </si>
   <si>
@@ -22728,37 +22716,13 @@
     <t>BS3 is a plant specific promoter which is induced by the TALE AvrBS3. The promoter is a useful tool in testing a system in which protein expression is activated in response to plant cell infection (in this case represented by presence of AvrBS3).</t>
   </si>
   <si>
-    <t>BBa_K1467102</t>
-  </si>
-  <si>
-    <t>PDF 1.2</t>
-  </si>
-  <si>
     <t>Source = BBa_K1467103, Golden Gate compatible</t>
   </si>
   <si>
-    <t>BBa_K1467103</t>
-  </si>
-  <si>
     <t>PDF 1.2 is a plant specific promoter which is induced by the compound Methyl Jasmonate - produced naturally by plants in response to various biotic and abiotic stresses such as wounding and pathogen infection. For this reason, the PDF1.2 promoter is useful for testing a system in which protein expression is initiated in response to pathogen infection (represented by the presence of methyl jasmonate).</t>
   </si>
   <si>
     <t>MAS (Mannopine synthase) is a plant specific promoter which is constitutively expressed. This part is compatible with the GoldenGate MoClo Assembly Standard as it is free from internal BsaI and BpiI recognition sequences.</t>
-  </si>
-  <si>
-    <t>Source = BBa_K1467104, Golden Gate compatible</t>
-  </si>
-  <si>
-    <t>BBa_K1467104</t>
-  </si>
-  <si>
-    <t>CaMV 35S</t>
-  </si>
-  <si>
-    <t>BS3</t>
-  </si>
-  <si>
-    <t>MAS</t>
   </si>
   <si>
     <t>AtU6</t>
@@ -22781,9 +22745,6 @@
     </r>
   </si>
   <si>
-    <t>CaMV 35S, BS3, PDF 1.2, MAS, AtU6</t>
-  </si>
-  <si>
     <t>hph</t>
   </si>
   <si>
@@ -22791,6 +22752,153 @@
   </si>
   <si>
     <t>Plant CDSs</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>CDS that confers BASTA resistnace</t>
+  </si>
+  <si>
+    <t>pSB1C5</t>
+  </si>
+  <si>
+    <t>NPTII</t>
+  </si>
+  <si>
+    <t>CDS that confers resistance to neomycin/kanamycij</t>
+  </si>
+  <si>
+    <t>SYnthetic</t>
+  </si>
+  <si>
+    <t>GFP</t>
+  </si>
+  <si>
+    <t>Codon-optimized for plants</t>
+  </si>
+  <si>
+    <t>Pnos</t>
+  </si>
+  <si>
+    <t>promoter of nopaline synthase, from A. tumefaciens</t>
+  </si>
+  <si>
+    <t>OCS</t>
+  </si>
+  <si>
+    <t>Plant terminators</t>
+  </si>
+  <si>
+    <t>Tnos</t>
+  </si>
+  <si>
+    <t>mCherry</t>
+  </si>
+  <si>
+    <t>RUBY</t>
+  </si>
+  <si>
+    <t>RUBY reporter for plant transformation</t>
+  </si>
+  <si>
+    <t>hph, Bar, NPTII, GFP, mCherry, RUBY</t>
+  </si>
+  <si>
+    <t>T35S</t>
+  </si>
+  <si>
+    <t>35S terminator</t>
+  </si>
+  <si>
+    <t>AtRbcS2B</t>
+  </si>
+  <si>
+    <t>OCS, Tnos, T35S</t>
+  </si>
+  <si>
+    <t>TMV_SV40</t>
+  </si>
+  <si>
+    <t>signal peptide for nuclear localization and enhanced translation</t>
+  </si>
+  <si>
+    <t>TMV_chloroplast_transit</t>
+  </si>
+  <si>
+    <t>signal peptide for chloroplast transport/localization</t>
+  </si>
+  <si>
+    <t>TMV</t>
+  </si>
+  <si>
+    <t>TMV enhancer of translation</t>
+  </si>
+  <si>
+    <t>P_LHB1B2</t>
+  </si>
+  <si>
+    <t>Plant 5UTRS</t>
+  </si>
+  <si>
+    <t>AtRbcS2B_UTR</t>
+  </si>
+  <si>
+    <t>AtRbcS2B_proUTR</t>
+  </si>
+  <si>
+    <t>CMV1_UTR</t>
+  </si>
+  <si>
+    <t>P_LHB1B2_UTR</t>
+  </si>
+  <si>
+    <t>CaMV35S</t>
+  </si>
+  <si>
+    <t>MAS_pro</t>
+  </si>
+  <si>
+    <t>BS3_proUTR</t>
+  </si>
+  <si>
+    <t>PDF1.2_pro</t>
+  </si>
+  <si>
+    <t>CaMV35S, BS3_proUTR, PDF1.2_pro, MAS_pro, AtU6, Pnos, AtRbcS2B_proUTR, P_LHB1B2</t>
+  </si>
+  <si>
+    <t>D1001</t>
+  </si>
+  <si>
+    <t>D1002</t>
+  </si>
+  <si>
+    <t>D1003</t>
+  </si>
+  <si>
+    <t>D1004</t>
+  </si>
+  <si>
+    <t>D1005</t>
+  </si>
+  <si>
+    <t>D1006</t>
+  </si>
+  <si>
+    <t>D1007</t>
+  </si>
+  <si>
+    <t>D1008</t>
+  </si>
+  <si>
+    <t>CMV1_UTR, AtRbcS2B_UTR, TMV, TMV_SV40, TMV_chloroplast_transit</t>
+  </si>
+  <si>
+    <t>Nikolaos Delkis, Rene Inckemann</t>
+  </si>
+  <si>
+    <t>This collection contains useful parts (promoters, UTRs, CDSs, terminators) for plant genetic engineering</t>
   </si>
 </sst>
 </file>
@@ -23158,7 +23266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23225,6 +23333,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23433,7 +23545,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M38" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M46" headerRowCount="0">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -23459,7 +23571,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A13:O20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_3" displayName="Table_3" ref="A13:O21">
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Part/Library Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Design Notes"/>
@@ -23682,7 +23794,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -23720,7 +23832,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7533</v>
+        <v>7593</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -23757,7 +23869,7 @@
     </row>
     <row r="5" spans="1:13" ht="45.95" customHeight="1">
       <c r="A5" s="53" t="s">
-        <v>7536</v>
+        <v>7594</v>
       </c>
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
@@ -24009,29 +24121,25 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="41" t="s">
-        <v>7549</v>
+        <v>7579</v>
       </c>
       <c r="B15" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>7535</v>
-      </c>
+      <c r="C15" s="41"/>
       <c r="D15" s="41" t="s">
         <v>1397</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>7538</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>42</v>
+        <v>7534</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>7521</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>7534</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>7417</v>
-      </c>
+        <v>7579</v>
+      </c>
+      <c r="H15" s="41"/>
       <c r="I15" s="41" t="s">
         <v>7417</v>
       </c>
@@ -24049,29 +24157,27 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
       <c r="A16" s="49" t="s">
-        <v>7550</v>
+        <v>7581</v>
       </c>
       <c r="B16" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>7539</v>
+        <v>7535</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>1397</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>7540</v>
+        <v>7536</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>42</v>
+        <v>7521</v>
       </c>
       <c r="G16" s="52" t="s">
-        <v>7541</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>7417</v>
-      </c>
+        <v>7581</v>
+      </c>
+      <c r="H16" s="41"/>
       <c r="I16" s="41" t="s">
         <v>7417</v>
       </c>
@@ -24089,29 +24195,27 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="41" t="s">
-        <v>7542</v>
+        <v>7582</v>
       </c>
       <c r="B17" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>7543</v>
+        <v>7537</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>1397</v>
       </c>
       <c r="E17" s="50" t="s">
-        <v>7545</v>
+        <v>7538</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>7544</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>7417</v>
-      </c>
+        <v>7521</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>7582</v>
+      </c>
+      <c r="H17" s="41"/>
       <c r="I17" s="41" t="s">
         <v>7417</v>
       </c>
@@ -24129,29 +24233,25 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
       <c r="A18" s="41" t="s">
-        <v>7551</v>
+        <v>7580</v>
       </c>
       <c r="B18" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="41" t="s">
-        <v>7547</v>
-      </c>
+      <c r="C18" s="41"/>
       <c r="D18" s="20" t="s">
         <v>1397</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>7546</v>
+        <v>7539</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>42</v>
+        <v>7521</v>
       </c>
       <c r="G18" s="52" t="s">
-        <v>7548</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>7417</v>
-      </c>
+        <v>7580</v>
+      </c>
+      <c r="H18" s="41"/>
       <c r="I18" s="41" t="s">
         <v>7417</v>
       </c>
@@ -24169,27 +24269,25 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="41" t="s">
-        <v>7552</v>
+        <v>7540</v>
       </c>
       <c r="B19" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>7553</v>
+        <v>7541</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>1397</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>7554</v>
+        <v>7542</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="20" t="s">
-        <v>7552</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>7417</v>
-      </c>
+        <v>7540</v>
+      </c>
+      <c r="H19" s="41"/>
       <c r="I19" s="41" t="s">
         <v>7417</v>
       </c>
@@ -24207,27 +24305,25 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
       <c r="A20" s="41" t="s">
-        <v>7501</v>
+        <v>7548</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>53</v>
+        <v>4473</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="20" t="s">
         <v>1397</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>7501</v>
+        <v>7548</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>42</v>
+        <v>7521</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>7501</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>7417</v>
-      </c>
+        <v>7548</v>
+      </c>
+      <c r="H20" s="41"/>
       <c r="I20" s="18" t="s">
         <v>7420</v>
       </c>
@@ -24245,7 +24341,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1">
       <c r="A21" s="41" t="s">
-        <v>7556</v>
+        <v>7543</v>
       </c>
       <c r="B21" s="41" t="s">
         <v>47</v>
@@ -24255,15 +24351,13 @@
         <v>1397</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>7557</v>
+        <v>7544</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="41" t="s">
-        <v>7556</v>
-      </c>
-      <c r="H21" s="41" t="s">
-        <v>7417</v>
-      </c>
+        <v>7543</v>
+      </c>
+      <c r="H21" s="41"/>
       <c r="I21" s="41" t="s">
         <v>7417</v>
       </c>
@@ -24280,15 +24374,29 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="18" t="s">
+        <v>7546</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="18" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>7547</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>7546</v>
+      </c>
       <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="I22" s="18" t="s">
+        <v>7417</v>
+      </c>
       <c r="J22" s="18" t="b">
         <v>0</v>
       </c>
@@ -24302,15 +24410,29 @@
       <c r="M22" s="18"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="18" t="s">
+        <v>7549</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="18" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>7550</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>7549</v>
+      </c>
       <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="I23" s="18" t="s">
+        <v>7551</v>
+      </c>
       <c r="J23" s="18" t="b">
         <v>0</v>
       </c>
@@ -24324,15 +24446,29 @@
       <c r="M23" s="18"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
+      <c r="A24" s="18" t="s">
+        <v>7552</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="C24" s="18"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="20"/>
+      <c r="D24" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>7553</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>7552</v>
+      </c>
       <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="I24" s="18" t="s">
+        <v>7417</v>
+      </c>
       <c r="J24" s="18" t="b">
         <v>0</v>
       </c>
@@ -24346,15 +24482,29 @@
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="18" t="s">
+        <v>7554</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="C25" s="18"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="20"/>
+      <c r="D25" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>7555</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>7554</v>
+      </c>
       <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="I25" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J25" s="18" t="b">
         <v>0</v>
       </c>
@@ -24368,15 +24518,27 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="41" t="s">
+        <v>7556</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>1783</v>
+      </c>
       <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="D26" s="41" t="s">
+        <v>1397</v>
+      </c>
       <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="F26" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>7556</v>
+      </c>
       <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="I26" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J26" s="18" t="b">
         <v>0</v>
       </c>
@@ -24390,15 +24552,27 @@
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
+      <c r="A27" s="41" t="s">
+        <v>7558</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>1783</v>
+      </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="20"/>
+      <c r="D27" s="20" t="s">
+        <v>1397</v>
+      </c>
       <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="F27" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>7558</v>
+      </c>
       <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="I27" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J27" s="18" t="b">
         <v>0</v>
       </c>
@@ -24412,15 +24586,27 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A28" s="41"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="41" t="s">
+        <v>7577</v>
+      </c>
+      <c r="B28" s="41" t="s">
+        <v>152</v>
+      </c>
       <c r="C28" s="18"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="20" t="s">
+        <v>1397</v>
+      </c>
       <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="F28" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>7577</v>
+      </c>
       <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="I28" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J28" s="18" t="b">
         <v>0</v>
       </c>
@@ -24434,15 +24620,29 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="41" t="s">
+        <v>7559</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>7553</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>7559</v>
+      </c>
       <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
+      <c r="I29" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J29" s="18" t="b">
         <v>0</v>
       </c>
@@ -24456,15 +24656,29 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A30" s="41"/>
-      <c r="B30" s="18"/>
+      <c r="A30" s="41" t="s">
+        <v>7560</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="C30" s="21"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="20"/>
+      <c r="D30" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>7561</v>
+      </c>
+      <c r="F30" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>7560</v>
+      </c>
       <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+      <c r="I30" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J30" s="18" t="b">
         <v>0</v>
       </c>
@@ -24478,15 +24692,29 @@
       <c r="M30" s="23"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A31" s="41"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="41" t="s">
+        <v>7563</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>1783</v>
+      </c>
       <c r="C31" s="18"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="20"/>
+      <c r="D31" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>7564</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>7563</v>
+      </c>
       <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+      <c r="I31" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J31" s="18" t="b">
         <v>0</v>
       </c>
@@ -24500,15 +24728,27 @@
       <c r="M31" s="23"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A32" s="41"/>
-      <c r="B32" s="18"/>
+      <c r="A32" s="41" t="s">
+        <v>7576</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="C32" s="18"/>
-      <c r="D32" s="20"/>
+      <c r="D32" s="20" t="s">
+        <v>1397</v>
+      </c>
       <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="20"/>
+      <c r="F32" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>7576</v>
+      </c>
       <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
+      <c r="I32" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J32" s="18" t="b">
         <v>0</v>
       </c>
@@ -24522,15 +24762,29 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A33" s="41"/>
-      <c r="B33" s="18"/>
+      <c r="A33" s="41" t="s">
+        <v>7567</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>104</v>
+      </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="20"/>
+      <c r="D33" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>7568</v>
+      </c>
+      <c r="F33" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>7567</v>
+      </c>
       <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
+      <c r="I33" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J33" s="18" t="b">
         <v>0</v>
       </c>
@@ -24544,15 +24798,29 @@
       <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A34" s="41"/>
-      <c r="B34" s="18"/>
+      <c r="A34" s="41" t="s">
+        <v>7569</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>104</v>
+      </c>
       <c r="C34" s="18"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="20"/>
+      <c r="D34" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>7570</v>
+      </c>
+      <c r="F34" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>7569</v>
+      </c>
       <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
+      <c r="I34" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J34" s="18" t="b">
         <v>0</v>
       </c>
@@ -24566,15 +24834,29 @@
       <c r="M34" s="21"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A35" s="41"/>
-      <c r="B35" s="18"/>
+      <c r="A35" s="41" t="s">
+        <v>7571</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>152</v>
+      </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="20"/>
+      <c r="D35" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>7572</v>
+      </c>
+      <c r="F35" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>7571</v>
+      </c>
       <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
+      <c r="I35" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J35" s="18" t="b">
         <v>0</v>
       </c>
@@ -24588,15 +24870,27 @@
       <c r="M35" s="21"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A36" s="41"/>
-      <c r="B36" s="18"/>
+      <c r="A36" s="41" t="s">
+        <v>7573</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>41</v>
+      </c>
       <c r="C36" s="18"/>
-      <c r="D36" s="20"/>
+      <c r="D36" s="20" t="s">
+        <v>1397</v>
+      </c>
       <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="20"/>
+      <c r="F36" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>7578</v>
+      </c>
       <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
+      <c r="I36" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J36" s="18" t="b">
         <v>0</v>
       </c>
@@ -24610,15 +24904,27 @@
       <c r="M36" s="21"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A37" s="41"/>
-      <c r="B37" s="18"/>
+      <c r="A37" s="41" t="s">
+        <v>7575</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>152</v>
+      </c>
       <c r="C37" s="18"/>
-      <c r="D37" s="20"/>
+      <c r="D37" s="20" t="s">
+        <v>1397</v>
+      </c>
       <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="20"/>
+      <c r="F37" s="41" t="s">
+        <v>7521</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>7565</v>
+      </c>
       <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
+      <c r="I37" s="41" t="s">
+        <v>7417</v>
+      </c>
       <c r="J37" s="18" t="b">
         <v>0</v>
       </c>
@@ -24632,15 +24938,27 @@
       <c r="M37" s="21"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A38" s="41"/>
-      <c r="B38" s="18"/>
+      <c r="A38" s="56" t="s">
+        <v>7584</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>1356</v>
+      </c>
       <c r="C38" s="18"/>
-      <c r="D38" s="20"/>
+      <c r="D38" s="20" t="s">
+        <v>1397</v>
+      </c>
       <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="20"/>
+      <c r="F38" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>7584</v>
+      </c>
       <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+      <c r="I38" s="18" t="s">
+        <v>7419</v>
+      </c>
       <c r="J38" s="18" t="b">
         <v>0</v>
       </c>
@@ -24653,14 +24971,266 @@
       </c>
       <c r="M38" s="21"/>
     </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A39" s="56" t="s">
+        <v>7585</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" s="56" t="s">
+        <v>7585</v>
+      </c>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39" s="15">
+        <f t="shared" ref="L39:L46" si="1">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M39,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="49"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A40" s="56" t="s">
+        <v>7586</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E40" s="18"/>
+      <c r="F40" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G40" s="56" t="s">
+        <v>7586</v>
+      </c>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J40" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L40" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="49"/>
+    </row>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A41" s="41" t="s">
+        <v>7587</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="41" t="s">
+        <v>7587</v>
+      </c>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J41" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="49"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A42" s="56" t="s">
+        <v>7588</v>
+      </c>
+      <c r="B42" s="41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" s="56" t="s">
+        <v>7588</v>
+      </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J42" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="49"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A43" s="41" t="s">
+        <v>7589</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E43" s="18"/>
+      <c r="F43" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="41" t="s">
+        <v>7589</v>
+      </c>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J43" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="49"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A44" s="41" t="s">
+        <v>7590</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E44" s="18"/>
+      <c r="F44" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="41" t="s">
+        <v>7590</v>
+      </c>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J44" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L44" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="49"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A45" s="41" t="s">
+        <v>7591</v>
+      </c>
+      <c r="B45" s="41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="20" t="s">
+        <v>1397</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" s="41" t="s">
+        <v>7591</v>
+      </c>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18" t="s">
+        <v>7419</v>
+      </c>
+      <c r="J45" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L45" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="49"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A46" s="41"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L46" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="49"/>
+    </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="48" spans="1:13" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
@@ -25614,31 +26184,31 @@
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F38</xm:sqref>
+          <xm:sqref>F15:F46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:I38</xm:sqref>
+          <xm:sqref>H15:I46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:B38</xm:sqref>
+          <xm:sqref>B15:B46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Sequence_alteration_terms!$A$2:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D38</xm:sqref>
+          <xm:sqref>D15:D46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J15:K38</xm:sqref>
+          <xm:sqref>J15:K46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25651,7 +26221,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -26145,21 +26715,25 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="49" t="s">
-        <v>7537</v>
+        <v>7533</v>
       </c>
       <c r="B14" s="21"/>
       <c r="D14" s="21" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>7501</v>
+        <v>7548</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="49" t="s">
-        <v>7555</v>
-      </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="32"/>
+      <c r="G14" s="56" t="s">
+        <v>7584</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>7583</v>
+      </c>
+      <c r="I14" s="56" t="s">
+        <v>7585</v>
+      </c>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -26177,23 +26751,27 @@
       <c r="X14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75">
-      <c r="A15" t="s">
-        <v>7558</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18" t="b">
+      <c r="A15" s="49" t="s">
+        <v>7574</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>7501</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18" t="s">
-        <v>7556</v>
-      </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="18"/>
+      <c r="E15" s="41" t="s">
+        <v>7548</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="49" t="s">
+        <v>7586</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>7592</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>7587</v>
+      </c>
       <c r="J15" s="18"/>
       <c r="K15" s="20"/>
       <c r="L15" s="18"/>
@@ -26211,16 +26789,27 @@
       <c r="X15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="B16" s="18"/>
+      <c r="A16" t="s">
+        <v>7545</v>
+      </c>
+      <c r="B16" s="21"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18"/>
+      <c r="D16" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>7548</v>
+      </c>
       <c r="F16" s="18"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="32"/>
+      <c r="G16" s="49" t="s">
+        <v>7588</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>7562</v>
+      </c>
+      <c r="I16" s="57" t="s">
+        <v>7589</v>
+      </c>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -26238,16 +26827,27 @@
       <c r="X16" s="3"/>
     </row>
     <row r="17" spans="1:25" ht="15" customHeight="1">
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="32"/>
+      <c r="A17" s="49" t="s">
+        <v>7557</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>7548</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="49" t="s">
+        <v>7590</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>7566</v>
+      </c>
+      <c r="I17" s="57" t="s">
+        <v>7591</v>
+      </c>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -26265,15 +26865,15 @@
       <c r="X17" s="3"/>
     </row>
     <row r="18" spans="1:25">
+      <c r="A18" s="49"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="32"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
@@ -26292,14 +26892,9 @@
       <c r="X18" s="3"/>
     </row>
     <row r="19" spans="1:25">
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40" t="b">
+      <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" s="40"/>
       <c r="J19" s="18"/>
@@ -26319,15 +26914,6 @@
       <c r="X19" s="3"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
       <c r="J20" s="18"/>
@@ -26360,7 +26946,7 @@
           <x14:formula1>
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D14:D16</xm:sqref>
+          <xm:sqref>D14 D16:D17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -26375,7 +26961,9 @@
   </sheetPr>
   <dimension ref="A1:M2535"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -26803,7 +27391,7 @@
       <c r="A25" s="3">
         <v>100</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="41" t="s">
         <v>152</v>
       </c>
       <c r="C25" s="3" t="s">

</xml_diff>

<commit_message>
Remove flanking seqs to see if fix
</commit_message>
<xml_diff>
--- a/Plant Parts/Plant Parts.xlsx
+++ b/Plant Parts/Plant Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\iGEM-distribution_2\Plant Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4E0CB-E8F5-4541-A4BA-370172E1DC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C9DE30-07CC-4DCF-8275-FBCDFB169323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="4800" windowWidth="32640" windowHeight="18330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7792" uniqueCount="7594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7784" uniqueCount="7594">
   <si>
     <t>Collection Name</t>
   </si>
@@ -23791,7 +23791,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="A42" sqref="A42:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -26217,8 +26217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -26722,15 +26722,10 @@
         <v>7548</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="53" t="s">
-        <v>7581</v>
-      </c>
-      <c r="H14" s="49" t="s">
+      <c r="G14" s="49" t="s">
         <v>7593</v>
       </c>
-      <c r="I14" s="53" t="s">
-        <v>7582</v>
-      </c>
+      <c r="I14" s="53"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -26760,15 +26755,10 @@
         <v>7548</v>
       </c>
       <c r="F15" s="40"/>
-      <c r="G15" s="49" t="s">
-        <v>7583</v>
-      </c>
-      <c r="H15" s="41" t="s">
+      <c r="G15" s="41" t="s">
         <v>7589</v>
       </c>
-      <c r="I15" s="41" t="s">
-        <v>7584</v>
-      </c>
+      <c r="I15" s="41"/>
       <c r="J15" s="18"/>
       <c r="K15" s="20"/>
       <c r="L15" s="18"/>
@@ -26798,15 +26788,10 @@
         <v>7548</v>
       </c>
       <c r="F16" s="18"/>
-      <c r="G16" s="49" t="s">
-        <v>7585</v>
-      </c>
-      <c r="H16" s="41" t="s">
+      <c r="G16" s="41" t="s">
         <v>7562</v>
       </c>
-      <c r="I16" s="54" t="s">
-        <v>7586</v>
-      </c>
+      <c r="I16" s="54"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -26837,14 +26822,9 @@
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="49" t="s">
-        <v>7587</v>
-      </c>
-      <c r="H17" s="49" t="s">
         <v>7566</v>
       </c>
-      <c r="I17" s="54" t="s">
-        <v>7588</v>
-      </c>
+      <c r="I17" s="54"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>

</xml_diff>

<commit_message>
Include 5-3UTRs in libraries sheet
</commit_message>
<xml_diff>
--- a/Plant Parts/Plant Parts.xlsx
+++ b/Plant Parts/Plant Parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\iGEM-distribution_2\Plant Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55909621-5C9C-472B-9C2F-FD390838CD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41688D7E-6BAF-4A6C-B513-D6E21CBCB577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7782" uniqueCount="7590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7792" uniqueCount="7595">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22884,6 +22884,21 @@
   </si>
   <si>
     <t>CaMV35S, BS3_proUTR, PDF1.2_pro, MAS_pro, AtU6, Pnos, AtRbcS2B_proUTR, LHB1B2_promoter</t>
+  </si>
+  <si>
+    <t>Plant fiveUTRs</t>
+  </si>
+  <si>
+    <t>Plant threeUTRs</t>
+  </si>
+  <si>
+    <t>CaMV35S_3UTR</t>
+  </si>
+  <si>
+    <t>TMV, TMV_chloroplast_transit, TMV_SV40, CMV1_UTR, AtRbcS2B_UTR</t>
+  </si>
+  <si>
+    <t>CaMV35S_3UTR, Tnos, OCS</t>
   </si>
 </sst>
 </file>
@@ -23779,7 +23794,7 @@
   <dimension ref="A1:M983"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="B27" activeCellId="1" sqref="B31 B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -24678,7 +24693,7 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1">
       <c r="A31" s="41" t="s">
-        <v>7562</v>
+        <v>7592</v>
       </c>
       <c r="B31" s="41" t="s">
         <v>1783</v>
@@ -26206,7 +26221,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -26773,16 +26788,27 @@
       <c r="X15" s="18"/>
     </row>
     <row r="16" spans="1:26" s="21" customFormat="1">
-      <c r="A16" s="49"/>
+      <c r="A16" s="49" t="s">
+        <v>7590</v>
+      </c>
       <c r="B16" s="40"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>7548</v>
+      </c>
       <c r="F16" s="40"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="32"/>
+      <c r="G16" s="21" t="s">
+        <v>7580</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>7593</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>7581</v>
+      </c>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -26800,16 +26826,27 @@
       <c r="X16" s="18"/>
     </row>
     <row r="17" spans="1:25" s="21" customFormat="1">
-      <c r="A17" s="49"/>
+      <c r="A17" s="49" t="s">
+        <v>7591</v>
+      </c>
       <c r="B17" s="40"/>
       <c r="C17" s="40"/>
       <c r="D17" s="40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>7548</v>
+      </c>
       <c r="F17" s="40"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="32"/>
+      <c r="G17" s="21" t="s">
+        <v>7584</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>7594</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>7585</v>
+      </c>
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>

</xml_diff>

<commit_message>
small fixes - added in pSB1C5.gb files to packages that need it, added flanking (buffer) regions for several small parts, edited OpenYeast to make Final Product as false (for now)
</commit_message>
<xml_diff>
--- a/Plant Parts/Plant Parts.xlsx
+++ b/Plant Parts/Plant Parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\iGEM-distribution_2\Plant Parts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Plant Parts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04D7D8D-066B-46FB-8D09-58850D445F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C8B3CA-B565-124A-A440-53A5E7A28D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33780" yWindow="-1260" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7792" uniqueCount="7595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7804" uniqueCount="7598">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22900,12 +22900,21 @@
   <si>
     <t>TMV, TMV_chloroplast_transit, TMV_SV40, CMV1_UTR, AtRbcS2B_5UTR</t>
   </si>
+  <si>
+    <t>D2001</t>
+  </si>
+  <si>
+    <t>Extra nonsense bases for synthesis</t>
+  </si>
+  <si>
+    <t>D2002</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23108,6 +23117,10 @@
       <color rgb="FF282828"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -23545,7 +23558,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M46" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M48" headerRowCount="0">
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -23793,24 +23806,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-    <col min="10" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" customWidth="1"/>
-    <col min="13" max="13" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="11" width="8.42578125" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
@@ -23867,7 +23880,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="45.95" customHeight="1">
+    <row r="5" spans="1:13" ht="46" customHeight="1">
       <c r="A5" s="55" t="s">
         <v>7586</v>
       </c>
@@ -25210,14 +25223,26 @@
       <c r="M45" s="49"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="41"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
+      <c r="A46" s="41" t="s">
+        <v>7595</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>7596</v>
+      </c>
       <c r="D46" s="20"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="18"/>
+      <c r="F46" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>7595</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>7417</v>
+      </c>
       <c r="I46" s="18"/>
       <c r="J46" s="18" t="b">
         <v>0</v>
@@ -25231,8 +25256,62 @@
       </c>
       <c r="M46" s="49"/>
     </row>
-    <row r="47" spans="1:13" ht="15.75" customHeight="1"/>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1"/>
+    <row r="47" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A47" s="41" t="s">
+        <v>7597</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>7596</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>7597</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>7417</v>
+      </c>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L47" s="15">
+        <f t="shared" ref="L47:L48" si="2">LEN(TRIM(CLEAN(SUBSTITUTE(SUBSTITUTE(M47,CHAR(160)," ")," ",""))))</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="49"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1">
+      <c r="A48" s="41"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L48" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="49"/>
+    </row>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -26172,6 +26251,7 @@
   <mergeCells count="1">
     <mergeCell ref="A5:F5"/>
   </mergeCells>
+  <phoneticPr fontId="31" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -26184,31 +26264,31 @@
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F46</xm:sqref>
+          <xm:sqref>F15:F48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$34</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:I46</xm:sqref>
+          <xm:sqref>H15:I48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:B46</xm:sqref>
+          <xm:sqref>B15:B48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Sequence_alteration_terms!$A$2:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D46</xm:sqref>
+          <xm:sqref>D15:D48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>'Ontology Terms'!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J15:K46</xm:sqref>
+          <xm:sqref>J15:K48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -26220,26 +26300,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="12" width="20.88671875" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="15" width="8.6640625" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" customWidth="1"/>
-    <col min="17" max="26" width="8.6640625" customWidth="1"/>
+    <col min="7" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="15" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="17" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75">
+    <row r="1" spans="1:26" ht="16">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -26268,7 +26348,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75">
+    <row r="2" spans="1:26" ht="16">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -26297,7 +26377,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3" spans="1:26" s="21" customFormat="1">
+    <row r="3" spans="1:26" s="21" customFormat="1" ht="16">
       <c r="A3" s="12" t="s">
         <v>7500</v>
       </c>
@@ -26334,7 +26414,7 @@
       <c r="X3" s="18"/>
       <c r="Y3" s="18"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="16">
       <c r="A4" s="12" t="s">
         <v>56</v>
       </c>
@@ -26373,7 +26453,7 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="16">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -26412,7 +26492,7 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="16">
       <c r="A6" s="12" t="s">
         <v>61</v>
       </c>
@@ -26447,7 +26527,7 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="16">
       <c r="A7" s="12" t="s">
         <v>63</v>
       </c>
@@ -26490,7 +26570,7 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="16">
       <c r="A8" s="12" t="s">
         <v>66</v>
       </c>
@@ -26555,7 +26635,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75">
+    <row r="10" spans="1:26" ht="16">
       <c r="A10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>68</v>
@@ -26584,7 +26664,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75">
+    <row r="11" spans="1:26" ht="16">
       <c r="A11" s="10" t="s">
         <v>7511</v>
       </c>
@@ -26750,7 +26830,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:26" s="21" customFormat="1">
+    <row r="15" spans="1:26" s="21" customFormat="1" ht="17">
       <c r="A15" s="21" t="s">
         <v>7545</v>
       </c>
@@ -26787,7 +26867,7 @@
       <c r="W15" s="18"/>
       <c r="X15" s="18"/>
     </row>
-    <row r="16" spans="1:26" s="21" customFormat="1">
+    <row r="16" spans="1:26" s="21" customFormat="1" ht="17">
       <c r="A16" s="49" t="s">
         <v>7589</v>
       </c>
@@ -26825,7 +26905,7 @@
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
     </row>
-    <row r="17" spans="1:25" s="21" customFormat="1">
+    <row r="17" spans="1:25" s="21" customFormat="1" ht="17">
       <c r="A17" s="49" t="s">
         <v>7590</v>
       </c>
@@ -26863,7 +26943,7 @@
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" ht="16">
       <c r="A18" s="49"/>
       <c r="B18" s="40"/>
       <c r="C18" s="40"/>
@@ -26890,7 +26970,7 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" ht="16">
       <c r="D19" t="b">
         <v>0</v>
       </c>
@@ -26912,7 +26992,7 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" ht="16">
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
       <c r="J20" s="18"/>
@@ -26964,11 +27044,11 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="26" width="10.5546875" customWidth="1"/>
+    <col min="3" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
@@ -69516,14 +69596,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
@@ -71509,9 +71589,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
@@ -72605,14 +72685,14 @@
       <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
@@ -75879,10 +75959,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">

</xml_diff>